<commit_message>
All three sentences works.
</commit_message>
<xml_diff>
--- a/part1/grammars/docs/grammar_drafts.xlsx
+++ b/part1/grammars/docs/grammar_drafts.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzotabasso/Desktop/University/TLN/Progetto/19-20/tln-1920/part1/grammars/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183F3D9B-6A6F-E44B-8B0E-332CF8F4B626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C63034-99E1-644C-8FC8-9436F452B86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5140" windowWidth="37200" windowHeight="21140" activeTab="1" xr2:uid="{2F2147DA-0289-444C-86DB-011EAE15B994}"/>
+    <workbookView xWindow="-37340" yWindow="-5140" windowWidth="37340" windowHeight="21140" xr2:uid="{2F2147DA-0289-444C-86DB-011EAE15B994}"/>
   </bookViews>
   <sheets>
-    <sheet name="Frasi" sheetId="2" r:id="rId1"/>
-    <sheet name="CFG 3 Frasi" sheetId="4" r:id="rId2"/>
-    <sheet name="CFG Work in Progress" sheetId="1" r:id="rId3"/>
+    <sheet name="CFG 3 Frasi" sheetId="4" r:id="rId1"/>
+    <sheet name="CFG Work in Progress" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>S -&gt; NP VP</t>
   </si>
@@ -196,19 +195,37 @@
     <t>VP -&gt; EX VBZ</t>
   </si>
   <si>
-    <t>VP -&gt; EX VBP</t>
-  </si>
-  <si>
     <t>VP -&gt; VBZ VBG</t>
   </si>
   <si>
-    <t>PP -&gt; IN IN RB</t>
-  </si>
-  <si>
     <t>PP -&gt; IN PP</t>
   </si>
   <si>
     <t>PP -&gt; PRP$ NN</t>
+  </si>
+  <si>
+    <t>NP -&gt; NN</t>
+  </si>
+  <si>
+    <t>PP -&gt; IN RB</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>ambiguità</t>
+  </si>
+  <si>
+    <t>Conta se usate</t>
+  </si>
+  <si>
+    <t>in frasi2</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -261,6 +278,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{774C0DCB-8257-CD46-A711-FC0A961265BF}" name="CFG3Frasi" displayName="CFG3Frasi" ref="A1:E15" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{944886B2-54DB-334A-B8EC-B419A4B19D9E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AAB899AB-BF3B-194F-9D0D-F31EADE47D93}" name="Regole"/>
+    <tableColumn id="2" xr3:uid="{79839D82-14E9-E343-AB40-0A2825F06C94}" name="Conta se usate"/>
+    <tableColumn id="3" xr3:uid="{9D8BB5C9-1DA9-1E4B-84EE-E431BFD0394E}" name="in frasi"/>
+    <tableColumn id="4" xr3:uid="{DEE5D23E-54CB-DF48-B2DE-E5BE9DB3DEEE}" name="in frasi2"/>
+    <tableColumn id="5" xr3:uid="{22C1B0A7-D398-4F41-9C18-A0AAA8BAC8E8}" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{85CA6F25-30E5-2447-B1AE-B65AC6EDAED7}" name="Frasi" displayName="Frasi" ref="G1:H13" totalsRowShown="0">
+  <autoFilter ref="G1:H13" xr:uid="{E99D3AE5-3D53-874E-9B85-CEAEA1E135E3}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CADEA5F8-CF03-8540-B550-8E7183598581}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{297823D5-78DD-C74A-B672-E8AC8FCC1F80}" name="Frasi"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,225 +610,320 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2486979C-E49B-3349-92E6-1B3091E760D2}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAA1F53-7833-974F-95D5-1ED03FE6BA76}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>55</v>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3476FE-4706-F541-8D48-11F9FFB0DFC4}">
   <dimension ref="A1:C40"/>
   <sheetViews>

</xml_diff>

<commit_message>
Mega commit: first and second sentence works, added Radisioni's part.
</commit_message>
<xml_diff>
--- a/part1/grammars/docs/grammar_drafts.xlsx
+++ b/part1/grammars/docs/grammar_drafts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzotabasso/Desktop/University/TLN/Progetto/19-20/tln-1920/part1/grammars/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C63034-99E1-644C-8FC8-9436F452B86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E76BCBB-F663-8C4D-8E3D-BBFF0CBBDC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37340" yWindow="-5140" windowWidth="37340" windowHeight="21140" xr2:uid="{2F2147DA-0289-444C-86DB-011EAE15B994}"/>
+    <workbookView xWindow="-37300" yWindow="-5140" windowWidth="37300" windowHeight="21140" xr2:uid="{2F2147DA-0289-444C-86DB-011EAE15B994}"/>
   </bookViews>
   <sheets>
     <sheet name="CFG 3 Frasi" sheetId="4" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>